<commit_message>
fix righe vuote excel
</commit_message>
<xml_diff>
--- a/prodotti.xlsx
+++ b/prodotti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmont\Desktop\Development\PrivateRepo\burgerpizzatemp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14995BB-1611-4067-8CC0-FF921A01D2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB35AC-29D6-4BCA-B6C7-A787983AB688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5475" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antipasti" sheetId="1" r:id="rId1"/>
@@ -857,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -878,10 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1187,7 +1184,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A17" sqref="A17:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015DF2A-0A06-4380-9DED-0895814E5B90}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,16 +1486,63 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>241</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-    </row>
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1507,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:XFD111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2108,9 +2152,6 @@
         <v>177</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2119,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A15" sqref="A15:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,9 +2368,6 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2340,7 +2378,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A4" sqref="A4:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>